<commit_message>
added sample name and cell dive id to sample annotations
</commit_message>
<xml_diff>
--- a/Cohort1/MetaData/MelanomaCohort1_SampleAnnotations.xlsx
+++ b/Cohort1/MetaData/MelanomaCohort1_SampleAnnotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\HaloData\Melanoma_IL2__Final\Cohort1\MetaData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Maryam\Analysis\Melanoma_IL2_Cohort1_v2\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Microscope</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>3_3RS</t>
+  </si>
+  <si>
+    <t>Sample_name</t>
+  </si>
+  <si>
+    <t>Untreated</t>
   </si>
 </sst>
 </file>
@@ -453,160 +459,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="19.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>2</v>
       </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>